<commit_message>
MALS-1104 resolve issues found during Demo
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://parcsystems.sharepoint.com/projects/Shared Documents/MALS/CDOGS/Development/MALS_Templates/Reports/Dairy-ClientDetails/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{17DF9D67-897B-4B5B-86B8-DEAA648C8A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{151E9ACE-CD06-404F-A478-A2DAC8ABA713}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E04CDC-71CF-43BF-9B55-19B8521DA07C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="-12800" windowWidth="23260" windowHeight="12580" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>{d.DateRangeEnd}</t>
   </si>
   <si>
-    <t>{d.Client[i]IRMA_NUM}</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -137,94 +134,97 @@
     <t>{d.Client[i].Status}</t>
   </si>
   <si>
-    <t>{d.Client[i]LicenceHolderCompany}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]LastnameFirstName}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]City} {d.Client[i]Province}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Address}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Postcode}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Phone}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Fax}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Cell}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Email}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]IssueDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]SiteAddress}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]SiteCity} {d.Client[i]SiteProvince}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]LastInspectionDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]LastInspector}</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
     <t>Details</t>
   </si>
   <si>
-    <t>{d.Client[i]TankCompany}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]TankModel}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]TankSerialNo}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]TankCapacity}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i]IH}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i]SCC}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i]IBC}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i]CRY}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Avg_IH}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Avg_SCC}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Avg_IBC}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Avg_CRY}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i]Date}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Insp[i+1]Date}</t>
+    <t>{d.Client[i].IRMA_Num}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].LicenceHolderCompany}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].LastnameFirstName}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Address}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Postcode}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].City} {d.Client[i].Province}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].IssueDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteAddress}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteCity} {d.Client[i].SiteProvince}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Phone}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Fax}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Cell}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Email}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankCompany}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankModel}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankCapacity}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].LastInspectionDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].LastInspector}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i].Date}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i+1].Date}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i].IH}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i].SCC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i].IBC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Insp[i].CRY}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Avg_IH}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Avg_SCC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Avg_IBC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Avg_CRY}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankSerial}</t>
   </si>
 </sst>
 </file>
@@ -334,12 +334,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +357,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,79 +680,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="135" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="J1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -762,12 +762,12 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -776,7 +776,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -786,7 +786,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -795,79 +795,79 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
-        <v>32</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>29</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
-        <v>30</v>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>31</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -877,27 +877,27 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>20</v>
@@ -912,59 +912,59 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
-        <v>30</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="15"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="7" t="s">
         <v>1</v>
@@ -979,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
@@ -996,62 +996,62 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="8"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
       <c r="C30" s="9"/>
@@ -1070,15 +1070,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1301,6 +1292,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1308,14 +1308,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2AF8CD6-3E38-48DB-89EE-EAD5D47F2F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1330,6 +1322,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix bad key name in template
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE3857-C63F-4DC2-8E86-2847AA3CAE87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A97CEBA-6D85-4FEC-BD4B-45D4EAB37661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>{d.Client[i].IRMA_Num}</t>
-  </si>
-  <si>
     <t>{d.Client[i].LicenceHolderCompany}</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>{d.Client[i].IRMA_NUM}</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="B1" s="10"/>
       <c r="F1" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G1" s="33"/>
       <c r="H1" s="33"/>
@@ -739,7 +739,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -767,7 +767,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -800,13 +800,13 @@
         <v>30</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="11"/>
@@ -818,13 +818,13 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="11"/>
@@ -836,13 +836,13 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
@@ -854,13 +854,13 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="11"/>
@@ -882,7 +882,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>32</v>
@@ -917,22 +917,22 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>33</v>
       </c>
       <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
         <v>48</v>
-      </c>
-      <c r="F18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -955,13 +955,13 @@
         <v>16</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,24 +998,24 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="D25" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="E25" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
@@ -1034,16 +1034,16 @@
         <v>18</v>
       </c>
       <c r="B28" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="D28" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="E28" s="32" t="s">
         <v>60</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1070,18 +1070,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1308,6 +1308,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137977AE-5CF3-42F0-AD7C-49AF06AF507F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1320,14 +1328,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add new variables (needs db changes)
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\Desktop\work\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ACE093-CB7E-42D5-82E6-13BEBEC43F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2C9FD6-F002-4465-A753-D17530B00761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>IH</t>
   </si>
@@ -231,6 +231,30 @@
   </si>
   <si>
     <t>Site Status:</t>
+  </si>
+  <si>
+    <t>Site ID</t>
+  </si>
+  <si>
+    <t>Tank #</t>
+  </si>
+  <si>
+    <t>Calibration Date</t>
+  </si>
+  <si>
+    <t>{d.Client[i].CalibrationDate}</t>
+  </si>
+  <si>
+    <t>Recheck Year</t>
+  </si>
+  <si>
+    <t>{d.Client[i].RecheckYear}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteId}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankId}</t>
   </si>
 </sst>
 </file>
@@ -282,43 +306,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -327,51 +337,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,7 +686,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,35 +697,35 @@
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="8" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="4"/>
+      <c r="F1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="J1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -747,7 +743,7 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -756,59 +752,59 @@
       <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -817,13 +813,13 @@
       <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
@@ -835,13 +831,13 @@
       <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
@@ -853,13 +849,13 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
@@ -871,45 +867,45 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -926,13 +922,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D18" t="s">
@@ -949,128 +945,134 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
+      <c r="A19" s="16"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="11"/>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B22" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="7" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B25" s="5">
         <v>0.15</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C25" s="4">
         <v>400000</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D25" s="4">
         <v>121000</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E25" s="5">
         <v>3.7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
+      <c r="B28" s="18"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B29" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C29" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D29" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E29" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1083,18 +1085,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1321,6 +1323,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137977AE-5CF3-42F0-AD7C-49AF06AF507F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1333,14 +1343,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
display all entries for given irma_number
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\Desktop\work\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2C9FD6-F002-4465-A753-D17530B00761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A99E064-5159-4112-A07D-322A8389B0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
     <t>IH</t>
   </si>
@@ -233,6 +233,198 @@
     <t>Site Status:</t>
   </si>
   <si>
+    <t>{d.Client[i+1].IRMA_NUM}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Status}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].LicenceHolderCompany}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].LastnameFirstName}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Phone}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Address}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Fax}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].City} {d.Client[i+1].Province}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Cell}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Postcode}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Email}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].IssueDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].SiteStatus}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].SiteAddress}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].SiteCity} {d.Client[i+1].SiteProvince}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].TankCompany}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].TankModel}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].TankSerial}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].TankCapacity}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].LastInspectionDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].LastInspector}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i].Date}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i].IH}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i].SCC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i].IBC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i].CRY}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Insp[i+1].Date}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Avg_IH}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Avg_SCC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Avg_IBC}</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].Avg_CRY}</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(IRMA:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(City / Province) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Site Address:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Site Status:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Date) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Report Average) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(IH) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(0.15) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Contact:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Client:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Site) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Details) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Make) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Model) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Serial #) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Capacity) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(SCC) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(IBC) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(CRY) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(400000) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(121000) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(3.7) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Last Inspected On:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Last Inspected By:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Email:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Cell:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Fax:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Phone:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Postcode) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Address) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Name) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Status:) }</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Issue Date:) }</t>
+  </si>
+  <si>
     <t>Site ID</t>
   </si>
   <si>
@@ -242,26 +434,50 @@
     <t>Calibration Date</t>
   </si>
   <si>
+    <t>Recheck Year</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteId}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].TankId}</t>
+  </si>
+  <si>
     <t>{d.Client[i].CalibrationDate}</t>
   </si>
   <si>
-    <t>Recheck Year</t>
-  </si>
-  <si>
     <t>{d.Client[i].RecheckYear}</t>
   </si>
   <si>
-    <t>{d.Client[i].SiteId}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].TankId}</t>
+    <t>{ d.Client[i+1]:ifNEM():show(Site ID) }</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].SiteId}</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Tank #) }</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].TankId}</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Calibration Date) }</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].CalibrationDate}</t>
+  </si>
+  <si>
+    <t>{ d.Client[i+1]:ifNEM():show(Recheck Year) }</t>
+  </si>
+  <si>
+    <t>{d.Client[i+1].RecheckYear}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +501,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,18 +528,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -363,6 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -683,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="135" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,35 +927,35 @@
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="10" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="F1" s="22" t="s">
+      <c r="B1" s="5"/>
+      <c r="F1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="J1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -743,7 +973,7 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -752,56 +982,56 @@
       <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
@@ -813,13 +1043,13 @@
       <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
@@ -831,13 +1061,13 @@
       <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
@@ -849,13 +1079,13 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
@@ -867,45 +1097,45 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="20" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -922,13 +1152,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="20" t="s">
         <v>33</v>
       </c>
       <c r="D18" t="s">
@@ -945,134 +1175,456 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="19"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="14"/>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E25" s="7" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="C25" s="4">
-        <v>400000</v>
-      </c>
-      <c r="D25" s="4">
-        <v>121000</v>
-      </c>
-      <c r="E25" s="5">
-        <v>3.7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="C26" s="5">
+        <v>400000</v>
+      </c>
+      <c r="D26" s="5">
+        <v>121000</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="18"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
+      <c r="B28" s="21"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="B29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B30" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C30" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D30" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E30" s="23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="3"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
+      <c r="D48" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="21"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="21"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1085,18 +1637,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1323,14 +1875,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137977AE-5CF3-42F0-AD7C-49AF06AF507F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1343,6 +1887,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
remove 4 new vars for now
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Client_Details_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\Desktop\work\nr-mals\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC5FBD3-837B-4B53-9410-2D5AA265E526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FCE2B3-C513-40AD-9C31-24B93A892015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>IH</t>
   </si>
@@ -423,54 +423,6 @@
   </si>
   <si>
     <t>{ d.Client[i+1]:ifNEM():show(Issue Date:) }</t>
-  </si>
-  <si>
-    <t>Site ID</t>
-  </si>
-  <si>
-    <t>Tank #</t>
-  </si>
-  <si>
-    <t>Calibration Date</t>
-  </si>
-  <si>
-    <t>Recheck Year</t>
-  </si>
-  <si>
-    <t>{d.Client[i].SiteId}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].TankId}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].CalibrationDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].RecheckYear}</t>
-  </si>
-  <si>
-    <t>{ d.Client[i+1]:ifNEM():show(Site ID) }</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].SiteId}</t>
-  </si>
-  <si>
-    <t>{ d.Client[i+1]:ifNEM():show(Tank #) }</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].TankId}</t>
-  </si>
-  <si>
-    <t>{ d.Client[i+1]:ifNEM():show(Calibration Date) }</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].CalibrationDate}</t>
-  </si>
-  <si>
-    <t>{ d.Client[i+1]:ifNEM():show(Recheck Year) }</t>
-  </si>
-  <si>
-    <t>{d.Client[i+1].RecheckYear}</t>
   </si>
 </sst>
 </file>
@@ -915,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,18 +1102,10 @@
       <c r="G17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
@@ -1184,18 +1128,6 @@
       </c>
       <c r="G18" t="s">
         <v>48</v>
-      </c>
-      <c r="H18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" t="s">
-        <v>135</v>
-      </c>
-      <c r="J18" t="s">
-        <v>136</v>
-      </c>
-      <c r="K18" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1480,18 +1412,10 @@
       <c r="G43" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>144</v>
-      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
@@ -1514,18 +1438,6 @@
       </c>
       <c r="G44" t="s">
         <v>84</v>
-      </c>
-      <c r="H44" t="s">
-        <v>139</v>
-      </c>
-      <c r="I44" t="s">
-        <v>141</v>
-      </c>
-      <c r="J44" t="s">
-        <v>143</v>
-      </c>
-      <c r="K44" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1637,18 +1549,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1875,14 +1787,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137977AE-5CF3-42F0-AD7C-49AF06AF507F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1895,6 +1799,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12EAFE4B-1F2D-4650-ACDE-3590E8305080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>